<commit_message>
Updated API Removed linting error
</commit_message>
<xml_diff>
--- a/documents/Published/Horizontal Funnel/HorizontalFunnelByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Horizontal Funnel/HorizontalFunnelByMAQSoftwareChecklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git1\documents\Published\Horizontal Funnel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual\documents\Published\Horizontal Funnel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61163D2-619C-4F6C-A9ED-4F9669BC5C4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C1D8AD-907C-45C3-A64F-E6D32200818F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4AB92824-63E9-41E2-A760-A81835BDCF59}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="110">
   <si>
     <t>S no</t>
   </si>
@@ -250,9 +250,6 @@
     <t>1. Go to formatting pane
 2. Go to Show Connectors 
 3. Update the show connectors button to 'OFF'</t>
-  </si>
-  <si>
-    <t>The value displayed on the tooltip should be same as actual data i.e. No formatting should be applied to the tooltip data</t>
   </si>
   <si>
     <t>Update color of labels</t>
@@ -439,6 +436,24 @@
   </si>
   <si>
     <t>Should display default text "Please select both 'Series' and 'Primary Measure' values"</t>
+  </si>
+  <si>
+    <t>PowerBi</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>The value displayed on the tooltip should be same as actual data i.e.No formatting should be applied to the tooltip data</t>
   </si>
 </sst>
 </file>
@@ -525,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -560,6 +575,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,6 +594,1815 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>108856</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>77892</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2163536</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1493328</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C0E6DF2-D18D-40CA-B34B-8946F1CE9D08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23295427" y="513321"/>
+          <a:ext cx="2054680" cy="1415436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>40820</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2277421</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1251857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79801A31-F31F-43F2-8B52-E306D68F93CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18764249" y="530679"/>
+          <a:ext cx="2236601" cy="1156607"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>122464</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>81055</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2073255</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1527381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D5B909C-F535-48D4-B41B-6251CCD4C365}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21186321" y="516484"/>
+          <a:ext cx="1950791" cy="1446326"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57897</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2054678</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1426019</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B39123A3-E8FE-4268-996C-AB8E9C99CB68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25091571" y="493326"/>
+          <a:ext cx="1973036" cy="1368122"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>34988</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2128765</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1333500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16B3BB3D-93FA-40CC-BF32-06726F130BEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25118786" y="2048845"/>
+          <a:ext cx="2019908" cy="1298512"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>81643</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90468</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2122715</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1401536</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B7CEA6-3A65-4142-8F90-DEF269C0C13B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23268214" y="2104325"/>
+          <a:ext cx="2041072" cy="1311068"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>40822</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2097810</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1369459</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEED1927-6638-40D8-BF93-F3222C846CED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21104679" y="2119697"/>
+          <a:ext cx="2056988" cy="1263619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>149678</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>119690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2261321</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1327368</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06F4CCBF-6DCF-42A5-88E5-585AFD307322}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18873107" y="2133547"/>
+          <a:ext cx="2111643" cy="1207678"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>40821</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>167020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2225784</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1543689</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBFC13DF-C5A3-4375-A065-4AF057158060}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23227392" y="3718484"/>
+          <a:ext cx="2184963" cy="1376669"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>107882</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2050123</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1340842</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F288C532-AC33-46D3-9738-2858AFA3E5EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25566846" y="3714750"/>
+          <a:ext cx="1942241" cy="1177556"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>159586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2108646</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1491937</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D35F7FFC-CB5D-4B88-8CE5-FF83DA326E9A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21159107" y="3711050"/>
+          <a:ext cx="2013396" cy="1332351"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>10431</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2187627</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1618590</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F083F4A-5405-4103-A561-F381C62D2068}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18733860" y="3578678"/>
+          <a:ext cx="2177196" cy="1591376"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>43948</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2470808</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1796143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{542F3F32-51E4-4320-9E0C-EAFC7E873CF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21107805" y="5279572"/>
+          <a:ext cx="2426860" cy="1741714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>54428</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>49194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2231572</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1734123</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B1A0D6-DCA8-4450-BAE0-CA1D2BF77CDE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23649214" y="5274337"/>
+          <a:ext cx="2177144" cy="1684929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>55599</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2141674</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1564821</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81E2CF80-F015-4644-BE26-A254DC7B2E46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25922778" y="5279571"/>
+          <a:ext cx="2086075" cy="1510393"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>68034</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>73865</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2193592</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1700893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85386F05-41A9-4BAB-A9AF-196BF6C2DB2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18791463" y="5299008"/>
+          <a:ext cx="2125558" cy="1627028"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>74541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2798213</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1728106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFED6805-6412-42C4-93A7-22AEA72BE945}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18805071" y="7299934"/>
+          <a:ext cx="2716571" cy="1653565"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>66708</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>122465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2567182</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1874317</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7283ED69-49C8-4EC8-869C-AC0DA62504C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26532601" y="7347858"/>
+          <a:ext cx="2500474" cy="1751852"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>40821</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>67832</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2653393</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1750420</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80FA0C23-CB1A-4260-BABB-D39BA2F41279}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24234321" y="7293225"/>
+          <a:ext cx="2612572" cy="1682588"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>109686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2479467</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1619249</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8839E4E6-5C94-4CE9-B074-89E582455B81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21730607" y="7335079"/>
+          <a:ext cx="2411431" cy="1509563"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2258785</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1401537</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F0640E5-6D44-4BC1-B64B-532155097F39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050000" y="9280072"/>
+          <a:ext cx="1932214" cy="1306286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>136070</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>144899</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2361709</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1470088</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B34754D-839C-417A-B862-F12605982767}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21798641" y="9329720"/>
+          <a:ext cx="2225639" cy="1325189"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>244929</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2231572</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1524000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9D47F0-A88D-4160-864E-821E349B5DA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24438429" y="9280071"/>
+          <a:ext cx="1986643" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>122463</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>103640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2721428</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1455965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAEE87F2-5B61-43C6-8A15-C82C5C3D51E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27023784" y="9288461"/>
+          <a:ext cx="2598965" cy="1352325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>204107</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2347531</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>968956</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1CD2E70-6AC8-44F6-A0EE-7808E73E3F99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18927536" y="11851821"/>
+          <a:ext cx="2143424" cy="914528"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>34530</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2870978</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1749242</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0583148D-59FF-4A03-88FA-74A0B0FA7669}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18757959" y="14586857"/>
+          <a:ext cx="2836448" cy="1667599"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>122978</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2367643</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1849738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD22C705-6D09-4E2E-BFFE-DD6E87A18FA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21785549" y="14614071"/>
+          <a:ext cx="2244665" cy="1740881"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>258285</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>54428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2462893</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1920543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{956A6E1E-FC33-4BFB-9DA3-F32211BFF12A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24451785" y="14559642"/>
+          <a:ext cx="2204608" cy="1866115"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>167155</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>108855</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2544536</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1834764</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F44D92D5-D00A-4E4B-B4AB-C92832FB1DDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27068476" y="14614069"/>
+          <a:ext cx="2377381" cy="1725909"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>639536</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>270099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2056536</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1478158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6FE3285-FAD8-4415-BB32-75193178B3C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19362965" y="19088778"/>
+          <a:ext cx="1417000" cy="1208059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>585108</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>160983</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2124330</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1728106</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE56059F-91EB-4E8D-8E54-D2F0761E47A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22247679" y="18979662"/>
+          <a:ext cx="1539222" cy="1567123"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>83952</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2587666</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1605643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4EA303-2BAF-414A-A60E-9E2B8ABEA500}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24277452" y="18981965"/>
+          <a:ext cx="2503714" cy="1442357"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>136072</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2394858</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>1634493</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20E11CA2-B764-43E9-92F0-B6E6AE0C8D2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27037393" y="18873108"/>
+          <a:ext cx="2258786" cy="1580064"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>802821</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>489857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2288928</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1366279</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{968A7D00-1943-4F7B-A8D0-A73292614E42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19526250" y="17498786"/>
+          <a:ext cx="1486107" cy="876422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>557892</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>639536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2348842</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1258747</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="Picture 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F187F774-97ED-4FA8-A3FA-5FD1725C8E32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27459213" y="17648465"/>
+          <a:ext cx="1790950" cy="619211"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>979714</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>680357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1713241</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1309095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FCF548C-890D-42C4-825C-6AF5C9012691}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25173214" y="17689286"/>
+          <a:ext cx="733527" cy="628738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1006929</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>789214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1607088</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1446531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F10DAFC-50A6-486B-B28C-23E87ADC8D7B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22669500" y="17798143"/>
+          <a:ext cx="600159" cy="657317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>305543</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>136069</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2041070</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1994180</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="Picture 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F283527-1940-4AFA-AF0F-E95137452532}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19028972" y="21145498"/>
+          <a:ext cx="1735527" cy="1858111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>734787</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2449287</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2106480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98EB19BE-A87D-4CEF-BC23-9F5ED4D84432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="27636108" y="21023036"/>
+          <a:ext cx="1714500" cy="2092873"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>353787</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1973037</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2054222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6CC59E-9ACA-4DCB-A39C-49CD3B7390E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="24547287" y="21172715"/>
+          <a:ext cx="1619250" cy="1890936"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>176893</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>13607</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1973036</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>17533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F99C34A8-723D-4DFC-8893-25CC881AC6B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="21839464" y="21023036"/>
+          <a:ext cx="1796143" cy="2167461"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -874,10 +2702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD979CE-A2F4-4A57-BF74-C680FEBF31B0}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,12 +2713,16 @@
     <col min="1" max="1" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="83.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="79.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="107.140625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="90.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="85.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="38" style="2" customWidth="1"/>
+    <col min="8" max="8" width="40.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="41.5703125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,8 +2738,20 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -921,10 +2765,22 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>37</v>
       </c>
@@ -935,7 +2791,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>38</v>
       </c>
@@ -946,7 +2802,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -963,7 +2819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
@@ -974,7 +2830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="154.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -982,7 +2838,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>51</v>
@@ -991,7 +2847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +2858,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1012,8 +2868,20 @@
       <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F9" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>4</v>
       </c>
@@ -1029,8 +2897,20 @@
       <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
@@ -1040,8 +2920,20 @@
       <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1051,8 +2943,17 @@
       <c r="E12" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="G12" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
@@ -1062,8 +2963,20 @@
       <c r="E13" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F13" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1073,8 +2986,20 @@
       <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1084,8 +3009,20 @@
       <c r="E15" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>5</v>
       </c>
@@ -1102,7 +3039,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -1118,8 +3055,20 @@
       <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F17" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>7</v>
       </c>
@@ -1132,11 +3081,11 @@
       <c r="D18" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" s="15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>8</v>
       </c>
@@ -1153,43 +3102,56 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
       <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
         <v>96</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="170.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>10</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1209,13 +3171,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1223,10 +3185,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1234,10 +3196,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,10 +3207,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1256,10 +3218,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1267,10 +3229,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1278,10 +3240,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1289,10 +3251,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1300,10 +3262,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1311,10 +3273,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1322,10 +3284,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1333,10 +3295,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1344,10 +3306,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1355,10 +3317,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1366,10 +3328,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1377,10 +3339,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1388,23 +3350,23 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="13"/>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C19" s="13"/>
     </row>
@@ -1413,10 +3375,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1424,23 +3386,23 @@
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" s="13"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="13"/>
     </row>
@@ -1452,7 +3414,7 @@
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="13"/>
     </row>
@@ -1461,10 +3423,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1472,10 +3434,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>